<commit_message>
design uppd 29e jan
</commit_message>
<xml_diff>
--- a/Design/designplanering1.xlsx
+++ b/Design/designplanering1.xlsx
@@ -830,7 +830,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="35" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="36" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="22" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="24" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="4" applyFont="1" applyBorder="1"/>
@@ -873,6 +872,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Accent1" xfId="4" builtinId="30"/>
@@ -1183,7 +1183,7 @@
   <dimension ref="A1:R45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1195,52 +1195,52 @@
     </row>
     <row r="2" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="32"/>
+      <c r="A3" s="31"/>
       <c r="B3" s="15"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="45" t="s">
+      <c r="C3" s="32"/>
+      <c r="D3" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="46">
+      <c r="E3" s="45">
         <v>1</v>
       </c>
-      <c r="F3" s="46">
+      <c r="F3" s="45">
         <v>2</v>
       </c>
-      <c r="G3" s="65">
+      <c r="G3" s="64">
         <v>3</v>
       </c>
-      <c r="H3" s="46">
+      <c r="H3" s="45">
         <v>4</v>
       </c>
-      <c r="I3" s="46">
+      <c r="I3" s="45">
         <v>5</v>
       </c>
-      <c r="J3" s="45">
+      <c r="J3" s="44">
         <v>6</v>
       </c>
-      <c r="K3" s="47">
+      <c r="K3" s="46">
         <v>7</v>
       </c>
-      <c r="L3" s="47">
+      <c r="L3" s="46">
         <v>8</v>
       </c>
-      <c r="M3" s="47">
+      <c r="M3" s="46">
         <v>9</v>
       </c>
-      <c r="N3" s="47">
+      <c r="N3" s="46">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="43" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="64"/>
+      <c r="D4" s="63"/>
       <c r="E4" s="17"/>
-      <c r="F4" s="18"/>
+      <c r="F4" s="70"/>
       <c r="G4" s="18"/>
       <c r="H4" s="18"/>
       <c r="I4" s="18"/>
@@ -1251,14 +1251,14 @@
       <c r="N4" s="19"/>
       <c r="O4">
         <f>(L6+J35)/2</f>
-        <v>26.666666666666671</v>
+        <v>31.666666666666668</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
-      <c r="D5" s="60"/>
+      <c r="D5" s="59"/>
       <c r="E5" s="21"/>
       <c r="F5" s="21"/>
       <c r="G5" s="21"/>
@@ -1268,17 +1268,17 @@
       <c r="K5" s="21"/>
       <c r="L5" s="16"/>
       <c r="M5" s="16"/>
-      <c r="N5" s="35"/>
+      <c r="N5" s="34"/>
     </row>
     <row r="6" spans="1:18" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="55" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
-      <c r="D6" s="59"/>
+      <c r="D6" s="58"/>
       <c r="E6" s="17"/>
-      <c r="F6" s="18"/>
+      <c r="F6" s="70"/>
       <c r="G6" s="18"/>
       <c r="H6" s="18"/>
       <c r="I6" s="18" t="s">
@@ -1286,18 +1286,18 @@
       </c>
       <c r="J6" s="18"/>
       <c r="K6" s="19"/>
-      <c r="L6" s="34">
+      <c r="L6" s="33">
         <f>(G8+G13+H18+J23+L28)/5</f>
-        <v>40.000000000000007</v>
+        <v>50</v>
       </c>
       <c r="M6" s="16"/>
-      <c r="N6" s="35"/>
+      <c r="N6" s="34"/>
     </row>
     <row r="7" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="13"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
-      <c r="D7" s="60"/>
+      <c r="D7" s="59"/>
       <c r="E7" s="21"/>
       <c r="F7" s="21"/>
       <c r="G7" s="16"/>
@@ -1310,15 +1310,15 @@
       <c r="N7" s="10"/>
     </row>
     <row r="8" spans="1:18" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="41" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
-      <c r="D8" s="61"/>
+      <c r="D8" s="60"/>
       <c r="E8" s="22"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="49">
+      <c r="F8" s="66"/>
+      <c r="G8" s="48">
         <f>(G9+G10+G11)/3</f>
         <v>100</v>
       </c>
@@ -1329,8 +1329,8 @@
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
       <c r="N8" s="10"/>
-      <c r="P8" s="70"/>
-      <c r="R8" s="70"/>
+      <c r="P8" s="69"/>
+      <c r="R8" s="69"/>
     </row>
     <row r="9" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
@@ -1338,7 +1338,7 @@
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
-      <c r="D9" s="61"/>
+      <c r="D9" s="60"/>
       <c r="E9" s="17"/>
       <c r="F9" s="27"/>
       <c r="G9" s="20">
@@ -1358,7 +1358,7 @@
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
-      <c r="D10" s="61"/>
+      <c r="D10" s="60"/>
       <c r="E10" s="25"/>
       <c r="F10" s="26"/>
       <c r="G10" s="20">
@@ -1371,7 +1371,7 @@
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
       <c r="N10" s="10"/>
-      <c r="P10" s="70"/>
+      <c r="P10" s="69"/>
     </row>
     <row r="11" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
@@ -1379,10 +1379,10 @@
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
-      <c r="D11" s="61"/>
+      <c r="D11" s="60"/>
       <c r="E11" s="25"/>
       <c r="F11" s="26"/>
-      <c r="G11" s="49">
+      <c r="G11" s="48">
         <v>100</v>
       </c>
       <c r="H11" s="9"/>
@@ -1392,13 +1392,13 @@
       <c r="L11" s="9"/>
       <c r="M11" s="9"/>
       <c r="N11" s="10"/>
-      <c r="P11" s="70"/>
+      <c r="P11" s="69"/>
     </row>
     <row r="12" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="14"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
-      <c r="D12" s="60"/>
+      <c r="D12" s="59"/>
       <c r="E12" s="16"/>
       <c r="F12" s="21"/>
       <c r="G12" s="9"/>
@@ -1411,17 +1411,17 @@
       <c r="N12" s="10"/>
     </row>
     <row r="13" spans="1:18" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="41" t="s">
         <v>30</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
-      <c r="D13" s="60"/>
+      <c r="D13" s="59"/>
       <c r="E13" s="28"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="49">
+      <c r="F13" s="73"/>
+      <c r="G13" s="48">
         <f>(G14+G15+G16)/3</f>
-        <v>66.666666666666671</v>
+        <v>100</v>
       </c>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
@@ -1437,10 +1437,10 @@
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
-      <c r="D14" s="60"/>
+      <c r="D14" s="59"/>
       <c r="E14" s="28"/>
-      <c r="F14" s="68"/>
-      <c r="G14" s="49">
+      <c r="F14" s="67"/>
+      <c r="G14" s="48">
         <v>100</v>
       </c>
       <c r="H14" s="9"/>
@@ -1457,10 +1457,10 @@
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="60"/>
+      <c r="D15" s="59"/>
       <c r="E15" s="28"/>
-      <c r="F15" s="69"/>
-      <c r="G15" s="49">
+      <c r="F15" s="68"/>
+      <c r="G15" s="48">
         <v>100</v>
       </c>
       <c r="H15" s="9"/>
@@ -1477,11 +1477,11 @@
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
-      <c r="D16" s="60"/>
+      <c r="D16" s="59"/>
       <c r="E16" s="28"/>
-      <c r="F16" s="30"/>
+      <c r="F16" s="68"/>
       <c r="G16" s="20">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
@@ -1495,7 +1495,7 @@
       <c r="A17" s="13"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
-      <c r="D17" s="60"/>
+      <c r="D17" s="59"/>
       <c r="E17" s="9"/>
       <c r="F17" s="16"/>
       <c r="G17" s="9"/>
@@ -1508,18 +1508,18 @@
       <c r="N17" s="10"/>
     </row>
     <row r="18" spans="1:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="42" t="s">
+      <c r="A18" s="41" t="s">
         <v>31</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
-      <c r="D18" s="60"/>
+      <c r="D18" s="59"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="G18" s="29"/>
       <c r="H18" s="9">
         <f>(H19+H20+H21)/3</f>
-        <v>33.333333333333336</v>
+        <v>50</v>
       </c>
       <c r="I18" s="9"/>
       <c r="J18" s="9"/>
@@ -1534,12 +1534,12 @@
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
-      <c r="D19" s="60"/>
+      <c r="D19" s="59"/>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
-      <c r="G19" s="31"/>
+      <c r="G19" s="67"/>
       <c r="H19" s="9">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
@@ -1554,12 +1554,12 @@
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
-      <c r="D20" s="60"/>
+      <c r="D20" s="59"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="G20" s="30"/>
       <c r="H20" s="9">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="I20" s="9"/>
       <c r="J20" s="9"/>
@@ -1574,7 +1574,7 @@
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="60"/>
+      <c r="D21" s="59"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="30"/>
@@ -1592,7 +1592,7 @@
       <c r="A22" s="14"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
-      <c r="D22" s="60"/>
+      <c r="D22" s="59"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -1605,16 +1605,16 @@
       <c r="N22" s="10"/>
     </row>
     <row r="23" spans="1:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="42" t="s">
+      <c r="A23" s="41" t="s">
         <v>18</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
-      <c r="D23" s="60"/>
+      <c r="D23" s="59"/>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
-      <c r="H23" s="39"/>
+      <c r="H23" s="38"/>
       <c r="I23" s="23"/>
       <c r="J23" s="9">
         <f>(J24+J25+J26)/3</f>
@@ -1631,11 +1631,11 @@
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
-      <c r="D24" s="60"/>
+      <c r="D24" s="59"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
-      <c r="H24" s="40"/>
+      <c r="H24" s="39"/>
       <c r="I24" s="19"/>
       <c r="J24" s="9">
         <v>0</v>
@@ -1651,11 +1651,11 @@
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
-      <c r="D25" s="60"/>
+      <c r="D25" s="59"/>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
-      <c r="H25" s="41"/>
+      <c r="H25" s="40"/>
       <c r="I25" s="24"/>
       <c r="J25" s="9">
         <v>0</v>
@@ -1671,11 +1671,11 @@
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
-      <c r="D26" s="60"/>
+      <c r="D26" s="59"/>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
-      <c r="H26" s="41"/>
+      <c r="H26" s="40"/>
       <c r="I26" s="24"/>
       <c r="J26" s="9">
         <v>0</v>
@@ -1689,33 +1689,33 @@
       <c r="A27" s="13"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
-      <c r="D27" s="62"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
-      <c r="K27" s="37"/>
-      <c r="L27" s="37"/>
-      <c r="M27" s="37"/>
-      <c r="N27" s="50"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
+      <c r="K27" s="36"/>
+      <c r="L27" s="36"/>
+      <c r="M27" s="36"/>
+      <c r="N27" s="49"/>
     </row>
     <row r="28" spans="1:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="42" t="s">
         <v>24</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="60"/>
+      <c r="D28" s="59"/>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
       <c r="H28" s="9"/>
       <c r="I28" s="9"/>
-      <c r="J28" s="40"/>
+      <c r="J28" s="39"/>
       <c r="K28" s="19"/>
-      <c r="L28" s="51">
+      <c r="L28" s="50">
         <f>(L29+L30+L31+L32+L33)/5</f>
         <v>0</v>
       </c>
@@ -1728,15 +1728,15 @@
       </c>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
-      <c r="D29" s="60"/>
+      <c r="D29" s="59"/>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
       <c r="I29" s="9"/>
-      <c r="J29" s="40"/>
+      <c r="J29" s="39"/>
       <c r="K29" s="19"/>
-      <c r="L29" s="52">
+      <c r="L29" s="51">
         <v>0</v>
       </c>
       <c r="M29" s="9"/>
@@ -1748,35 +1748,35 @@
       </c>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
-      <c r="D30" s="60"/>
+      <c r="D30" s="59"/>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
-      <c r="J30" s="40"/>
+      <c r="J30" s="39"/>
       <c r="K30" s="19"/>
-      <c r="L30" s="51">
+      <c r="L30" s="50">
         <v>0</v>
       </c>
       <c r="M30" s="9"/>
       <c r="N30" s="10"/>
     </row>
     <row r="31" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="54" t="s">
+      <c r="A31" s="53" t="s">
         <v>27</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="60"/>
+      <c r="D31" s="59"/>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
       <c r="I31" s="9"/>
-      <c r="J31" s="40"/>
+      <c r="J31" s="39"/>
       <c r="K31" s="19"/>
-      <c r="L31" s="51">
+      <c r="L31" s="50">
         <v>0</v>
       </c>
       <c r="M31" s="9"/>
@@ -1788,35 +1788,35 @@
       </c>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
-      <c r="D32" s="60"/>
+      <c r="D32" s="59"/>
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
       <c r="H32" s="9"/>
       <c r="I32" s="9"/>
-      <c r="J32" s="40"/>
+      <c r="J32" s="39"/>
       <c r="K32" s="19"/>
-      <c r="L32" s="51">
+      <c r="L32" s="50">
         <v>0</v>
       </c>
       <c r="M32" s="9"/>
       <c r="N32" s="10"/>
     </row>
     <row r="33" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="54" t="s">
+      <c r="A33" s="53" t="s">
         <v>22</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
-      <c r="D33" s="60"/>
+      <c r="D33" s="59"/>
       <c r="E33" s="9"/>
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
       <c r="I33" s="9"/>
-      <c r="J33" s="40"/>
+      <c r="J33" s="39"/>
       <c r="K33" s="19"/>
-      <c r="L33" s="53">
+      <c r="L33" s="52">
         <v>0</v>
       </c>
       <c r="M33" s="9"/>
@@ -1826,12 +1826,12 @@
       <c r="A34" s="6"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
-      <c r="D34" s="60"/>
-      <c r="E34" s="37"/>
-      <c r="F34" s="37"/>
-      <c r="G34" s="37"/>
-      <c r="H34" s="37"/>
-      <c r="I34" s="37"/>
+      <c r="D34" s="59"/>
+      <c r="E34" s="36"/>
+      <c r="F34" s="36"/>
+      <c r="G34" s="36"/>
+      <c r="H34" s="36"/>
+      <c r="I34" s="36"/>
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
       <c r="L34" s="9"/>
@@ -1839,22 +1839,22 @@
       <c r="N34" s="10"/>
     </row>
     <row r="35" spans="1:14" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="48" t="s">
+      <c r="A35" s="47" t="s">
         <v>25</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="61"/>
+      <c r="D35" s="60"/>
       <c r="E35" s="17"/>
-      <c r="F35" s="71"/>
+      <c r="F35" s="70"/>
       <c r="G35" s="18"/>
       <c r="H35" s="18"/>
       <c r="I35" s="19"/>
-      <c r="J35" s="73">
+      <c r="J35" s="72">
         <f>(J37+J38)/3</f>
         <v>13.333333333333334</v>
       </c>
-      <c r="K35" s="72" t="s">
+      <c r="K35" s="71" t="s">
         <v>35</v>
       </c>
       <c r="L35" s="9"/>
@@ -1865,7 +1865,7 @@
       <c r="A36" s="6"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
-      <c r="D36" s="60"/>
+      <c r="D36" s="59"/>
       <c r="E36" s="21"/>
       <c r="F36" s="21"/>
       <c r="G36" s="21"/>
@@ -1883,13 +1883,13 @@
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="61"/>
+      <c r="D37" s="60"/>
       <c r="E37" s="17"/>
-      <c r="F37" s="71"/>
+      <c r="F37" s="70"/>
       <c r="G37" s="18"/>
       <c r="H37" s="18"/>
       <c r="I37" s="19"/>
-      <c r="J37" s="49">
+      <c r="J37" s="48">
         <v>40</v>
       </c>
       <c r="K37" s="9"/>
@@ -1903,11 +1903,11 @@
       </c>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
-      <c r="D38" s="60"/>
+      <c r="D38" s="59"/>
       <c r="E38" s="16"/>
       <c r="F38" s="16"/>
-      <c r="G38" s="58"/>
-      <c r="H38" s="40"/>
+      <c r="G38" s="57"/>
+      <c r="H38" s="39"/>
       <c r="I38" s="19"/>
       <c r="J38" s="20">
         <v>0</v>
@@ -1921,10 +1921,10 @@
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
-      <c r="D39" s="60"/>
+      <c r="D39" s="59"/>
       <c r="E39" s="9"/>
       <c r="F39" s="9"/>
-      <c r="G39" s="37"/>
+      <c r="G39" s="36"/>
       <c r="H39" s="21"/>
       <c r="I39" s="16"/>
       <c r="J39" s="9"/>
@@ -1934,17 +1934,17 @@
       <c r="N39" s="10"/>
     </row>
     <row r="40" spans="1:14" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="57" t="s">
+      <c r="A40" s="56" t="s">
         <v>34</v>
       </c>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
-      <c r="D40" s="60"/>
+      <c r="D40" s="59"/>
       <c r="E40" s="9"/>
       <c r="F40" s="28"/>
-      <c r="G40" s="38"/>
+      <c r="G40" s="37"/>
       <c r="H40" s="19"/>
-      <c r="I40" s="52">
+      <c r="I40" s="51">
         <f>I42</f>
         <v>0</v>
       </c>
@@ -1976,12 +1976,12 @@
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
-      <c r="D42" s="66"/>
+      <c r="D42" s="65"/>
       <c r="E42" s="16"/>
-      <c r="F42" s="58"/>
-      <c r="G42" s="40"/>
+      <c r="F42" s="57"/>
+      <c r="G42" s="39"/>
       <c r="H42" s="19"/>
-      <c r="I42" s="52">
+      <c r="I42" s="51">
         <f>(I43+I44+I45)/3</f>
         <v>0</v>
       </c>
@@ -1989,7 +1989,7 @@
       <c r="K42" s="16"/>
       <c r="L42" s="16"/>
       <c r="M42" s="16"/>
-      <c r="N42" s="35"/>
+      <c r="N42" s="34"/>
     </row>
     <row r="43" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="6" t="s">
@@ -1997,12 +1997,12 @@
       </c>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
-      <c r="D43" s="60"/>
+      <c r="D43" s="59"/>
       <c r="E43" s="9"/>
       <c r="F43" s="28"/>
-      <c r="G43" s="40"/>
+      <c r="G43" s="39"/>
       <c r="H43" s="19"/>
-      <c r="I43" s="51">
+      <c r="I43" s="50">
         <v>0</v>
       </c>
       <c r="J43" s="9"/>
@@ -2012,17 +2012,17 @@
       <c r="N43" s="10"/>
     </row>
     <row r="44" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="55" t="s">
+      <c r="A44" s="54" t="s">
         <v>8</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
-      <c r="D44" s="60"/>
+      <c r="D44" s="59"/>
       <c r="E44" s="9"/>
       <c r="F44" s="28"/>
-      <c r="G44" s="40"/>
+      <c r="G44" s="39"/>
       <c r="H44" s="19"/>
-      <c r="I44" s="51">
+      <c r="I44" s="50">
         <v>0</v>
       </c>
       <c r="J44" s="9"/>
@@ -2037,12 +2037,12 @@
       </c>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
-      <c r="D45" s="63"/>
+      <c r="D45" s="62"/>
       <c r="E45" s="11"/>
-      <c r="F45" s="36"/>
-      <c r="G45" s="40"/>
+      <c r="F45" s="35"/>
+      <c r="G45" s="39"/>
       <c r="H45" s="19"/>
-      <c r="I45" s="51">
+      <c r="I45" s="50">
         <v>0</v>
       </c>
       <c r="J45" s="11"/>

</xml_diff>